<commit_message>
Updated output files for ACR and SHS
Updated output files for ACR and SHS - CIFMM-2436.
</commit_message>
<xml_diff>
--- a/output/AdvanceCareRecords/composition-acp-1.xlsx
+++ b/output/AdvanceCareRecords/composition-acp-1.xlsx
@@ -174,7 +174,7 @@
     <t>Y</t>
   </si>
   <si>
-    <t xml:space="preserve">id {[]} {[]}
+    <t xml:space="preserve">id
 </t>
   </si>
   <si>
@@ -193,7 +193,7 @@
     <t>Composition.meta</t>
   </si>
   <si>
-    <t xml:space="preserve">Meta {[]} {[]}
+    <t xml:space="preserve">Meta
 </t>
   </si>
   <si>
@@ -213,7 +213,7 @@
     <t>Composition.meta.id</t>
   </si>
   <si>
-    <t xml:space="preserve">string {[]} {[]}
+    <t xml:space="preserve">string
 </t>
   </si>
   <si>
@@ -236,7 +236,7 @@
 user content</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {[]} {[]}
+    <t xml:space="preserve">Extension
 </t>
   </si>
   <si>
@@ -280,7 +280,7 @@
     <t>Composition.meta.lastUpdated</t>
   </si>
   <si>
-    <t xml:space="preserve">instant {[]} {[]}
+    <t xml:space="preserve">instant
 </t>
   </si>
   <si>
@@ -299,7 +299,7 @@
     <t>Composition.meta.profile</t>
   </si>
   <si>
-    <t xml:space="preserve">uri {[]} {[]}
+    <t xml:space="preserve">uri
 </t>
   </si>
   <si>
@@ -318,7 +318,7 @@
     <t>Composition.meta.security</t>
   </si>
   <si>
-    <t xml:space="preserve">Coding {[]} {[]}
+    <t xml:space="preserve">Coding
 </t>
   </si>
   <si>
@@ -386,7 +386,7 @@
     <t>Composition.language</t>
   </si>
   <si>
-    <t xml:space="preserve">code {[]} {[]}
+    <t xml:space="preserve">code
 </t>
   </si>
   <si>
@@ -399,7 +399,7 @@
     <t>Language is provided to support indexing and accessibility (typically, services such as text to speech use the language tag). The html language tag in the narrative applies  to the narrative. The language tag on the resource may be used to specify the language of other presentations generated from the data in the resource  Not all the content has to be in the base language. The Resource.language should not be assumed to apply to the narrative automatically. If a language is specified, it should it also be specified on the div element in the html (see rules in HTML5 for information about the relationship between xml:lang and the html lang attribute).</t>
   </si>
   <si>
-    <t>&lt;valueCode xmlns="http://hl7.org/fhir" value="en-AU"/&gt;</t>
+    <t>en-AU</t>
   </si>
   <si>
     <t>A human language.</t>
@@ -418,7 +418,7 @@
 htmlxhtmldisplay</t>
   </si>
   <si>
-    <t xml:space="preserve">Narrative {[]} {[]}
+    <t xml:space="preserve">Narrative
 </t>
   </si>
   <si>
@@ -448,7 +448,7 @@
 anonymous resourcescontained resources</t>
   </si>
   <si>
-    <t xml:space="preserve">Resource {[]} {[]}
+    <t xml:space="preserve">Resource
 </t>
   </si>
   <si>
@@ -482,7 +482,7 @@
     <t>compositionAuthorRole</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {[CanonicalType[http://hl7.org.au/fhir/StructureDefinition/composition-author-role]]} {[]}
+    <t xml:space="preserve">Extension {http://hl7.org.au/fhir/StructureDefinition/composition-author-role}
 </t>
   </si>
   <si>
@@ -503,7 +503,7 @@
     <t>informationRecipient</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {[CanonicalType[http://hl7.org.au/fhir/StructureDefinition/information-recipient]]} {[]}
+    <t xml:space="preserve">Extension {http://hl7.org.au/fhir/StructureDefinition/information-recipient}
 </t>
   </si>
   <si>
@@ -532,7 +532,7 @@
     <t>Composition.identifier</t>
   </si>
   <si>
-    <t xml:space="preserve">Identifier {[]} {[]}
+    <t xml:space="preserve">Identifier
 </t>
   </si>
   <si>
@@ -588,7 +588,7 @@
     <t>Composition.type</t>
   </si>
   <si>
-    <t xml:space="preserve">CodeableConcept {[]} {[]}
+    <t xml:space="preserve">CodeableConcept
 </t>
   </si>
   <si>
@@ -657,7 +657,7 @@
     <t>Composition.subject</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-ident-1]]}
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-ident-1)
 </t>
   </si>
   <si>
@@ -685,7 +685,7 @@
     <t>Composition.encounter</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Encounter]]}
+    <t xml:space="preserve">Reference(Encounter)
 </t>
   </si>
   <si>
@@ -710,7 +710,7 @@
     <t>Composition.date</t>
   </si>
   <si>
-    <t xml:space="preserve">dateTime {[]} {[]}
+    <t xml:space="preserve">dateTime
 </t>
   </si>
   <si>
@@ -738,7 +738,7 @@
     <t>Composition.author</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitioner-ident-1], CanonicalType[http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-ident-1], CanonicalType[http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/relatedperson-ident-1]]}
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitioner-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/relatedperson-ident-1)
 </t>
   </si>
   <si>
@@ -803,7 +803,7 @@
     <t>Composition.attester</t>
   </si>
   <si>
-    <t xml:space="preserve">BackboneElement {[]} {[]}
+    <t xml:space="preserve">BackboneElement
 </t>
   </si>
   <si>
@@ -838,7 +838,7 @@
     <t>attesterRelatedParty</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {[CanonicalType[http://hl7.org.au/fhir/StructureDefinition/attester-related-party]]} {[]}
+    <t xml:space="preserve">Extension {http://hl7.org.au/fhir/StructureDefinition/attester-related-party}
 </t>
   </si>
   <si>
@@ -870,7 +870,7 @@
     <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
   </si>
   <si>
-    <t>&lt;valueUri xmlns="http://hl7.org/fhir" value="http://hl7.org.au/fhir/StructureDefinition/attester-related-party"/&gt;</t>
+    <t>http://hl7.org.au/fhir/StructureDefinition/attester-related-party</t>
   </si>
   <si>
     <t>Extension.url</t>
@@ -882,7 +882,7 @@
     <t>valueReference</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org.au/fhir/StructureDefinition/attester-related-party]]}
+    <t xml:space="preserve">Reference(http://hl7.org.au/fhir/StructureDefinition/attester-related-party)
 </t>
   </si>
   <si>
@@ -923,7 +923,7 @@
     <t>Indicates the level of authority of the attestation.</t>
   </si>
   <si>
-    <t>&lt;valueCode xmlns="http://hl7.org/fhir" value="legal"/&gt;</t>
+    <t>legal</t>
   </si>
   <si>
     <t>The way in which a person authenticated a composition.</t>
@@ -959,7 +959,7 @@
     <t>Composition.attester.party</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-ident-1], CanonicalType[http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitioner-ident-1]]}
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitioner-ident-1)
 </t>
   </si>
   <si>
@@ -984,7 +984,7 @@
     <t>Composition.custodian</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/organization-ident-1]]}
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/organization-ident-1)
 </t>
   </si>
   <si>
@@ -1064,8 +1064,8 @@
     <t>Composition.relatesTo.target[x]</t>
   </si>
   <si>
-    <t>Identifier {[]} {[]}
-Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Composition]]}</t>
+    <t>Identifier
+Reference(Composition)</t>
   </si>
   <si>
     <t>Target of the relationship</t>
@@ -1131,7 +1131,7 @@
     <t>Composition.event.period</t>
   </si>
   <si>
-    <t xml:space="preserve">Period {[]} {[]}
+    <t xml:space="preserve">Period
 </t>
   </si>
   <si>
@@ -1144,7 +1144,7 @@
     <t>Composition.event.detail</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Resource]]}
+    <t xml:space="preserve">Reference(Resource)
 </t>
   </si>
   <si>
@@ -1185,7 +1185,7 @@
     <t>sectionAuthor</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {[CanonicalType[http://hl7.org.au/fhir/StructureDefinition/section-author]]} {[]}
+    <t xml:space="preserve">Extension {http://hl7.org.au/fhir/StructureDefinition/section-author}
 </t>
   </si>
   <si>
@@ -1316,7 +1316,7 @@
     <t>Composition.section.entry</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/documentreference-acp-1]]}
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/documentreference-acp-1)
 </t>
   </si>
   <si>
@@ -1428,67 +1428,67 @@
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin"/>
     </border>
     <border>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin"/>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <top style="thin"/>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </top>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="23"/>
       </bottom>
     </border>
   </borders>
@@ -1524,7 +1524,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AM68"/>
+  <dimension ref="A1:AL68"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>

</xml_diff>

<commit_message>
Regenerated output files CIFMM-2481
</commit_message>
<xml_diff>
--- a/output/AdvanceCareRecords/composition-acp-1.xlsx
+++ b/output/AdvanceCareRecords/composition-acp-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$64</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2313" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2178" uniqueCount="420">
   <si>
     <t>Path</t>
   </si>
@@ -497,7 +497,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}inv-dh-cmp-04:A practitioner role shall conform to PractitionerRole with Practitioner with Mandatory Identifier {Composition.extension('http://hl7.org.au/fhir/StructureDefinition/composition-author-role').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitioner-ident-1')}</t>
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}inv-dh-cmp-04:A practitioner role shall conform to PractitionerRole with Practitioner with Mandatory Identifier {Composition.extension('http://hl7.org.au/fhir/StructureDefinition/composition-author-role').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitioner-ident-1')}</t>
   </si>
   <si>
     <t>informationRecipient</t>
@@ -849,50 +849,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}inv-dh-cmp-05:A related party shall conform to RelatedPerson with Mandatory Identifier {Composition.attester.extension('http://hl7.org.au/fhir/StructureDefinition/attester-related-party').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/relatedperson-ident-1')}</t>
-  </si>
-  <si>
-    <t>Composition.attester.extension.id</t>
-  </si>
-  <si>
-    <t>Composition.attester.extension.extension</t>
-  </si>
-  <si>
-    <t>Composition.attester.extension.url</t>
-  </si>
-  <si>
-    <t>identifies the meaning of the extension</t>
-  </si>
-  <si>
-    <t>Source of the definition for the extension code - a logical name or a URL.</t>
-  </si>
-  <si>
-    <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
-  </si>
-  <si>
-    <t>http://hl7.org.au/fhir/StructureDefinition/attester-related-party</t>
-  </si>
-  <si>
-    <t>Extension.url</t>
-  </si>
-  <si>
-    <t>Composition.attester.extension.valueReference</t>
-  </si>
-  <si>
-    <t>valueReference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference(http://hl7.org.au/fhir/StructureDefinition/attester-related-party)
-</t>
-  </si>
-  <si>
-    <t>Value of extension</t>
-  </si>
-  <si>
-    <t>Value of extension - may be a resource or one of a constrained set of the data types (see Extensibility in the spec for list).</t>
-  </si>
-  <si>
-    <t>Extension.value[x]</t>
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}inv-dh-cmp-05:A related party shall conform to RelatedPerson with Mandatory Identifier {Composition.attester.extension('http://hl7.org.au/fhir/StructureDefinition/attester-related-party').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/relatedperson-ident-1')}</t>
   </si>
   <si>
     <t>Composition.attester.modifierExtension</t>
@@ -1524,7 +1481,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AL68"/>
+  <dimension ref="A1:AL64"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1533,7 +1490,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="43.73046875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="38.1328125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="22.32421875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
@@ -5149,34 +5106,36 @@
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>39</v>
+        <v>266</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F34" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G34" t="s" s="2">
         <v>39</v>
       </c>
       <c r="H34" t="s" s="2">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="I34" t="s" s="2">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>65</v>
+        <v>160</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>66</v>
-      </c>
-      <c r="M34" s="2"/>
+        <v>267</v>
+      </c>
+      <c r="M34" t="s" s="2">
+        <v>74</v>
+      </c>
       <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
         <v>39</v>
@@ -5225,13 +5184,13 @@
         <v>39</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>67</v>
+        <v>268</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG34" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AH34" t="s" s="2">
         <v>39</v>
@@ -5240,7 +5199,7 @@
         <v>39</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="AK34" t="s" s="2">
         <v>39</v>
@@ -5249,49 +5208,51 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" hidden="true">
+    <row r="35">
       <c r="A35" t="s" s="2">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F35" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G35" t="s" s="2">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="H35" t="s" s="2">
         <v>39</v>
       </c>
       <c r="I35" t="s" s="2">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>71</v>
+        <v>119</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>72</v>
+        <v>270</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>73</v>
+        <v>271</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="N35" s="2"/>
+        <v>272</v>
+      </c>
+      <c r="N35" t="s" s="2">
+        <v>273</v>
+      </c>
       <c r="O35" t="s" s="2">
         <v>39</v>
       </c>
       <c r="P35" s="2"/>
       <c r="Q35" t="s" s="2">
-        <v>39</v>
+        <v>274</v>
       </c>
       <c r="R35" t="s" s="2">
         <v>39</v>
@@ -5309,34 +5270,34 @@
         <v>39</v>
       </c>
       <c r="W35" t="s" s="2">
-        <v>39</v>
+        <v>176</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>39</v>
+        <v>275</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>39</v>
+        <v>276</v>
       </c>
       <c r="Z35" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AA35" t="s" s="2">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="AB35" t="s" s="2">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="AC35" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD35" t="s" s="2">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>78</v>
+        <v>269</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>41</v>
@@ -5348,18 +5309,18 @@
         <v>39</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>68</v>
+        <v>277</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>39</v>
+        <v>278</v>
       </c>
       <c r="AL35" t="s" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="36" hidden="true">
+    <row r="36">
       <c r="A36" t="s" s="2">
-        <v>267</v>
+        <v>279</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5373,33 +5334,33 @@
         <v>50</v>
       </c>
       <c r="G36" t="s" s="2">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="H36" t="s" s="2">
         <v>39</v>
       </c>
       <c r="I36" t="s" s="2">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>91</v>
+        <v>220</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>268</v>
+        <v>280</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>270</v>
-      </c>
-      <c r="N36" s="2"/>
+        <v>281</v>
+      </c>
+      <c r="M36" s="2"/>
+      <c r="N36" t="s" s="2">
+        <v>282</v>
+      </c>
       <c r="O36" t="s" s="2">
         <v>39</v>
       </c>
       <c r="P36" s="2"/>
       <c r="Q36" t="s" s="2">
-        <v>271</v>
+        <v>39</v>
       </c>
       <c r="R36" t="s" s="2">
         <v>39</v>
@@ -5441,10 +5402,10 @@
         <v>39</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>50</v>
@@ -5456,52 +5417,52 @@
         <v>39</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>143</v>
+        <v>283</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>39</v>
+        <v>284</v>
       </c>
       <c r="AL36" t="s" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="37" hidden="true">
+    <row r="37">
       <c r="A37" t="s" s="2">
-        <v>273</v>
-      </c>
-      <c r="B37" t="s" s="2">
-        <v>274</v>
-      </c>
+        <v>285</v>
+      </c>
+      <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
         <v>39</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F37" t="s" s="2">
         <v>50</v>
       </c>
       <c r="G37" t="s" s="2">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="H37" t="s" s="2">
         <v>39</v>
       </c>
       <c r="I37" t="s" s="2">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>275</v>
+        <v>286</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>276</v>
+        <v>287</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>277</v>
+        <v>288</v>
       </c>
       <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
+      <c r="N37" t="s" s="2">
+        <v>289</v>
+      </c>
       <c r="O37" t="s" s="2">
         <v>39</v>
       </c>
@@ -5549,7 +5510,7 @@
         <v>39</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>40</v>
@@ -5564,52 +5525,54 @@
         <v>39</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>143</v>
+        <v>290</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>39</v>
+        <v>291</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>39</v>
+        <v>292</v>
       </c>
     </row>
-    <row r="38" hidden="true">
+    <row r="38">
       <c r="A38" t="s" s="2">
-        <v>279</v>
+        <v>293</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
-        <v>280</v>
+        <v>39</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="H38" t="s" s="2">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="I38" t="s" s="2">
         <v>51</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>71</v>
+        <v>294</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>160</v>
+        <v>295</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>281</v>
+        <v>296</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="N38" s="2"/>
+        <v>297</v>
+      </c>
+      <c r="N38" t="s" s="2">
+        <v>298</v>
+      </c>
       <c r="O38" t="s" s="2">
         <v>39</v>
       </c>
@@ -5657,13 +5620,13 @@
         <v>39</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>282</v>
+        <v>293</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG38" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AH38" t="s" s="2">
         <v>39</v>
@@ -5672,18 +5635,18 @@
         <v>39</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>143</v>
+        <v>299</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>39</v>
+        <v>300</v>
       </c>
       <c r="AL38" t="s" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>283</v>
+        <v>301</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5691,13 +5654,13 @@
       </c>
       <c r="D39" s="2"/>
       <c r="E39" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G39" t="s" s="2">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="H39" t="s" s="2">
         <v>39</v>
@@ -5706,26 +5669,24 @@
         <v>51</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>119</v>
+        <v>250</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>284</v>
+        <v>302</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>285</v>
+        <v>303</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>286</v>
-      </c>
-      <c r="N39" t="s" s="2">
-        <v>287</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
         <v>39</v>
       </c>
       <c r="P39" s="2"/>
       <c r="Q39" t="s" s="2">
-        <v>288</v>
+        <v>39</v>
       </c>
       <c r="R39" t="s" s="2">
         <v>39</v>
@@ -5743,13 +5704,13 @@
         <v>39</v>
       </c>
       <c r="W39" t="s" s="2">
-        <v>176</v>
+        <v>39</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>289</v>
+        <v>39</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>290</v>
+        <v>39</v>
       </c>
       <c r="Z39" t="s" s="2">
         <v>39</v>
@@ -5767,10 +5728,10 @@
         <v>39</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>283</v>
+        <v>301</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>41</v>
@@ -5779,21 +5740,21 @@
         <v>39</v>
       </c>
       <c r="AI39" t="s" s="2">
-        <v>39</v>
+        <v>305</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>292</v>
+        <v>307</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>293</v>
+        <v>308</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5801,33 +5762,31 @@
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F40" t="s" s="2">
         <v>50</v>
       </c>
       <c r="G40" t="s" s="2">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="H40" t="s" s="2">
         <v>39</v>
       </c>
       <c r="I40" t="s" s="2">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>220</v>
+        <v>64</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>294</v>
+        <v>65</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>295</v>
+        <v>66</v>
       </c>
       <c r="M40" s="2"/>
-      <c r="N40" t="s" s="2">
-        <v>296</v>
-      </c>
+      <c r="N40" s="2"/>
       <c r="O40" t="s" s="2">
         <v>39</v>
       </c>
@@ -5875,7 +5834,7 @@
         <v>39</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>293</v>
+        <v>67</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>40</v>
@@ -5890,52 +5849,52 @@
         <v>39</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>297</v>
+        <v>68</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>298</v>
+        <v>39</v>
       </c>
       <c r="AL40" t="s" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>299</v>
+        <v>309</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G41" t="s" s="2">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="H41" t="s" s="2">
         <v>39</v>
       </c>
       <c r="I41" t="s" s="2">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>300</v>
+        <v>71</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>301</v>
+        <v>72</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>302</v>
-      </c>
-      <c r="M41" s="2"/>
-      <c r="N41" t="s" s="2">
-        <v>303</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="M41" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
         <v>39</v>
       </c>
@@ -5983,13 +5942,13 @@
         <v>39</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>299</v>
+        <v>78</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG41" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AH41" t="s" s="2">
         <v>39</v>
@@ -5998,54 +5957,52 @@
         <v>39</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>304</v>
+        <v>68</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>305</v>
+        <v>39</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>306</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
-        <v>39</v>
+        <v>266</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F42" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G42" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H42" t="s" s="2">
         <v>51</v>
-      </c>
-      <c r="H42" t="s" s="2">
-        <v>39</v>
       </c>
       <c r="I42" t="s" s="2">
         <v>51</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>308</v>
+        <v>71</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>309</v>
+        <v>160</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>310</v>
+        <v>267</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>311</v>
-      </c>
-      <c r="N42" t="s" s="2">
-        <v>312</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
         <v>39</v>
       </c>
@@ -6093,13 +6050,13 @@
         <v>39</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>307</v>
+        <v>268</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG42" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AH42" t="s" s="2">
         <v>39</v>
@@ -6108,10 +6065,10 @@
         <v>39</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>313</v>
+        <v>143</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>314</v>
+        <v>39</v>
       </c>
       <c r="AL42" t="s" s="2">
         <v>39</v>
@@ -6119,7 +6076,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6127,10 +6084,10 @@
       </c>
       <c r="D43" s="2"/>
       <c r="E43" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G43" t="s" s="2">
         <v>39</v>
@@ -6142,16 +6099,16 @@
         <v>51</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>250</v>
+        <v>119</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
@@ -6177,13 +6134,13 @@
         <v>39</v>
       </c>
       <c r="W43" t="s" s="2">
-        <v>39</v>
+        <v>176</v>
       </c>
       <c r="X43" t="s" s="2">
-        <v>39</v>
+        <v>315</v>
       </c>
       <c r="Y43" t="s" s="2">
-        <v>39</v>
+        <v>316</v>
       </c>
       <c r="Z43" t="s" s="2">
         <v>39</v>
@@ -6201,25 +6158,25 @@
         <v>39</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="AG43" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AH43" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>319</v>
+        <v>39</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="AL43" t="s" s="2">
         <v>39</v>
@@ -6227,7 +6184,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6235,7 +6192,7 @@
       </c>
       <c r="D44" s="2"/>
       <c r="E44" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F44" t="s" s="2">
         <v>50</v>
@@ -6247,16 +6204,16 @@
         <v>39</v>
       </c>
       <c r="I44" t="s" s="2">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>64</v>
+        <v>320</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>65</v>
+        <v>321</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>66</v>
+        <v>322</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -6307,10 +6264,10 @@
         <v>39</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>67</v>
+        <v>319</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>50</v>
@@ -6322,10 +6279,10 @@
         <v>39</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>68</v>
+        <v>323</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>39</v>
+        <v>324</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>39</v>
@@ -6333,11 +6290,11 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s" s="2">
@@ -6353,21 +6310,23 @@
         <v>39</v>
       </c>
       <c r="I45" t="s" s="2">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>71</v>
+        <v>250</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>72</v>
+        <v>326</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>73</v>
+        <v>327</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="N45" s="2"/>
+        <v>328</v>
+      </c>
+      <c r="N45" t="s" s="2">
+        <v>329</v>
+      </c>
       <c r="O45" t="s" s="2">
         <v>39</v>
       </c>
@@ -6415,7 +6374,7 @@
         <v>39</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>78</v>
+        <v>325</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>40</v>
@@ -6427,13 +6386,13 @@
         <v>39</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>39</v>
+        <v>305</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>68</v>
+        <v>330</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>39</v>
+        <v>331</v>
       </c>
       <c r="AL45" t="s" s="2">
         <v>39</v>
@@ -6441,40 +6400,38 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
-        <v>280</v>
+        <v>39</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G46" t="s" s="2">
         <v>39</v>
       </c>
       <c r="H46" t="s" s="2">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="I46" t="s" s="2">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>160</v>
+        <v>65</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>281</v>
-      </c>
-      <c r="M46" t="s" s="2">
-        <v>74</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="M46" s="2"/>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
         <v>39</v>
@@ -6523,13 +6480,13 @@
         <v>39</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>282</v>
+        <v>67</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG46" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AH46" t="s" s="2">
         <v>39</v>
@@ -6538,7 +6495,7 @@
         <v>39</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>143</v>
+        <v>68</v>
       </c>
       <c r="AK46" t="s" s="2">
         <v>39</v>
@@ -6549,18 +6506,18 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F47" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G47" t="s" s="2">
         <v>39</v>
@@ -6569,19 +6526,19 @@
         <v>39</v>
       </c>
       <c r="I47" t="s" s="2">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>119</v>
+        <v>71</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>326</v>
+        <v>72</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>327</v>
+        <v>73</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>328</v>
+        <v>74</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
@@ -6607,13 +6564,13 @@
         <v>39</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>176</v>
+        <v>39</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>329</v>
+        <v>39</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>330</v>
+        <v>39</v>
       </c>
       <c r="Z47" t="s" s="2">
         <v>39</v>
@@ -6631,13 +6588,13 @@
         <v>39</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>325</v>
+        <v>78</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="AG47" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AH47" t="s" s="2">
         <v>39</v>
@@ -6646,10 +6603,10 @@
         <v>39</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>331</v>
+        <v>68</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>332</v>
+        <v>39</v>
       </c>
       <c r="AL47" t="s" s="2">
         <v>39</v>
@@ -6657,38 +6614,40 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>39</v>
+        <v>266</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F48" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G48" t="s" s="2">
         <v>39</v>
       </c>
       <c r="H48" t="s" s="2">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="I48" t="s" s="2">
         <v>51</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>334</v>
+        <v>71</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>335</v>
+        <v>160</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>336</v>
-      </c>
-      <c r="M48" s="2"/>
+        <v>267</v>
+      </c>
+      <c r="M48" t="s" s="2">
+        <v>74</v>
+      </c>
       <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
         <v>39</v>
@@ -6737,13 +6696,13 @@
         <v>39</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>333</v>
+        <v>268</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="AG48" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AH48" t="s" s="2">
         <v>39</v>
@@ -6752,10 +6711,10 @@
         <v>39</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>337</v>
+        <v>143</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>338</v>
+        <v>39</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>39</v>
@@ -6763,7 +6722,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6786,20 +6745,18 @@
         <v>51</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>250</v>
+        <v>182</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>342</v>
-      </c>
-      <c r="N49" t="s" s="2">
-        <v>343</v>
-      </c>
+        <v>338</v>
+      </c>
+      <c r="N49" s="2"/>
       <c r="O49" t="s" s="2">
         <v>39</v>
       </c>
@@ -6823,13 +6780,13 @@
         <v>39</v>
       </c>
       <c r="W49" t="s" s="2">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>39</v>
+        <v>339</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>39</v>
+        <v>340</v>
       </c>
       <c r="Z49" t="s" s="2">
         <v>39</v>
@@ -6847,7 +6804,7 @@
         <v>39</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>40</v>
@@ -6859,13 +6816,13 @@
         <v>39</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>319</v>
+        <v>39</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>344</v>
+        <v>192</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>345</v>
+        <v>192</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>39</v>
@@ -6873,7 +6830,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6893,16 +6850,16 @@
         <v>39</v>
       </c>
       <c r="I50" t="s" s="2">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>64</v>
+        <v>342</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>65</v>
+        <v>343</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>66</v>
+        <v>344</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -6953,7 +6910,7 @@
         <v>39</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>67</v>
+        <v>341</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>40</v>
@@ -6968,10 +6925,10 @@
         <v>39</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>68</v>
+        <v>226</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>39</v>
+        <v>226</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>39</v>
@@ -6979,11 +6936,11 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
@@ -6999,20 +6956,18 @@
         <v>39</v>
       </c>
       <c r="I51" t="s" s="2">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>71</v>
+        <v>346</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>72</v>
+        <v>347</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>74</v>
-      </c>
+        <v>348</v>
+      </c>
+      <c r="M51" s="2"/>
       <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
         <v>39</v>
@@ -7061,7 +7016,7 @@
         <v>39</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>78</v>
+        <v>345</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>40</v>
@@ -7076,51 +7031,49 @@
         <v>39</v>
       </c>
       <c r="AJ51" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="AK51" t="s" s="2">
         <v>68</v>
       </c>
-      <c r="AK51" t="s" s="2">
-        <v>39</v>
-      </c>
       <c r="AL51" t="s" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="52" hidden="true">
+    <row r="52">
       <c r="A52" t="s" s="2">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
-        <v>280</v>
+        <v>39</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F52" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G52" t="s" s="2">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="H52" t="s" s="2">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="I52" t="s" s="2">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>71</v>
+        <v>250</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>160</v>
+        <v>351</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>281</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>74</v>
-      </c>
+        <v>352</v>
+      </c>
+      <c r="M52" s="2"/>
       <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
         <v>39</v>
@@ -7169,7 +7122,7 @@
         <v>39</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>282</v>
+        <v>350</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>40</v>
@@ -7181,13 +7134,13 @@
         <v>39</v>
       </c>
       <c r="AI52" t="s" s="2">
-        <v>39</v>
+        <v>353</v>
       </c>
       <c r="AJ52" t="s" s="2">
-        <v>143</v>
+        <v>354</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>39</v>
+        <v>355</v>
       </c>
       <c r="AL52" t="s" s="2">
         <v>39</v>
@@ -7195,7 +7148,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>349</v>
+        <v>356</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7206,7 +7159,7 @@
         <v>40</v>
       </c>
       <c r="F53" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G53" t="s" s="2">
         <v>39</v>
@@ -7215,20 +7168,18 @@
         <v>39</v>
       </c>
       <c r="I53" t="s" s="2">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>182</v>
+        <v>64</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>350</v>
+        <v>65</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>351</v>
-      </c>
-      <c r="M53" t="s" s="2">
-        <v>352</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="M53" s="2"/>
       <c r="N53" s="2"/>
       <c r="O53" t="s" s="2">
         <v>39</v>
@@ -7253,13 +7204,13 @@
         <v>39</v>
       </c>
       <c r="W53" t="s" s="2">
-        <v>109</v>
+        <v>39</v>
       </c>
       <c r="X53" t="s" s="2">
-        <v>353</v>
+        <v>39</v>
       </c>
       <c r="Y53" t="s" s="2">
-        <v>354</v>
+        <v>39</v>
       </c>
       <c r="Z53" t="s" s="2">
         <v>39</v>
@@ -7277,13 +7228,13 @@
         <v>39</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>349</v>
+        <v>67</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG53" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AH53" t="s" s="2">
         <v>39</v>
@@ -7292,10 +7243,10 @@
         <v>39</v>
       </c>
       <c r="AJ53" t="s" s="2">
-        <v>192</v>
+        <v>68</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>192</v>
+        <v>39</v>
       </c>
       <c r="AL53" t="s" s="2">
         <v>39</v>
@@ -7303,7 +7254,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7314,7 +7265,7 @@
         <v>40</v>
       </c>
       <c r="F54" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G54" t="s" s="2">
         <v>39</v>
@@ -7323,16 +7274,16 @@
         <v>39</v>
       </c>
       <c r="I54" t="s" s="2">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>356</v>
+        <v>71</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>357</v>
+        <v>145</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>358</v>
+        <v>146</v>
       </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -7371,25 +7322,23 @@
         <v>39</v>
       </c>
       <c r="AA54" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB54" t="s" s="2">
-        <v>39</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="AB54" s="2"/>
       <c r="AC54" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD54" t="s" s="2">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>355</v>
+        <v>78</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG54" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AH54" t="s" s="2">
         <v>39</v>
@@ -7398,10 +7347,10 @@
         <v>39</v>
       </c>
       <c r="AJ54" t="s" s="2">
-        <v>226</v>
+        <v>39</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>226</v>
+        <v>39</v>
       </c>
       <c r="AL54" t="s" s="2">
         <v>39</v>
@@ -7409,9 +7358,11 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>359</v>
-      </c>
-      <c r="B55" s="2"/>
+        <v>357</v>
+      </c>
+      <c r="B55" t="s" s="2">
+        <v>358</v>
+      </c>
       <c r="C55" t="s" s="2">
         <v>39</v>
       </c>
@@ -7429,16 +7380,16 @@
         <v>39</v>
       </c>
       <c r="I55" t="s" s="2">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="J55" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="K55" t="s" s="2">
         <v>360</v>
       </c>
-      <c r="K55" t="s" s="2">
+      <c r="L55" t="s" s="2">
         <v>361</v>
-      </c>
-      <c r="L55" t="s" s="2">
-        <v>362</v>
       </c>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -7489,7 +7440,7 @@
         <v>39</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>359</v>
+        <v>78</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>40</v>
@@ -7498,55 +7449,57 @@
         <v>41</v>
       </c>
       <c r="AH55" t="s" s="2">
-        <v>39</v>
+        <v>152</v>
       </c>
       <c r="AI55" t="s" s="2">
-        <v>39</v>
+        <v>158</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>363</v>
+        <v>39</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="AL55" t="s" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
-        <v>39</v>
+        <v>266</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F56" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H56" t="s" s="2">
         <v>51</v>
       </c>
-      <c r="H56" t="s" s="2">
-        <v>39</v>
-      </c>
       <c r="I56" t="s" s="2">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>250</v>
+        <v>71</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>365</v>
+        <v>160</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>366</v>
-      </c>
-      <c r="M56" s="2"/>
+        <v>267</v>
+      </c>
+      <c r="M56" t="s" s="2">
+        <v>74</v>
+      </c>
       <c r="N56" s="2"/>
       <c r="O56" t="s" s="2">
         <v>39</v>
@@ -7595,7 +7548,7 @@
         <v>39</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>364</v>
+        <v>268</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>40</v>
@@ -7607,35 +7560,35 @@
         <v>39</v>
       </c>
       <c r="AI56" t="s" s="2">
-        <v>367</v>
+        <v>39</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>368</v>
+        <v>143</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>369</v>
+        <v>39</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="57" hidden="true">
+    <row r="57">
       <c r="A57" t="s" s="2">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
-        <v>39</v>
+        <v>364</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F57" t="s" s="2">
         <v>50</v>
       </c>
       <c r="G57" t="s" s="2">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="H57" t="s" s="2">
         <v>39</v>
@@ -7647,13 +7600,17 @@
         <v>64</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>65</v>
+        <v>365</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>66</v>
-      </c>
-      <c r="M57" s="2"/>
-      <c r="N57" s="2"/>
+        <v>366</v>
+      </c>
+      <c r="M57" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="N57" t="s" s="2">
+        <v>368</v>
+      </c>
       <c r="O57" t="s" s="2">
         <v>39</v>
       </c>
@@ -7701,7 +7658,7 @@
         <v>39</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>67</v>
+        <v>363</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>40</v>
@@ -7716,18 +7673,18 @@
         <v>39</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>68</v>
+        <v>240</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>39</v>
+        <v>241</v>
       </c>
       <c r="AL57" t="s" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="58" hidden="true">
+    <row r="58">
       <c r="A58" t="s" s="2">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7735,13 +7692,13 @@
       </c>
       <c r="D58" s="2"/>
       <c r="E58" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F58" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G58" t="s" s="2">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="H58" t="s" s="2">
         <v>39</v>
@@ -7750,22 +7707,26 @@
         <v>39</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>71</v>
+        <v>182</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>145</v>
+        <v>370</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>146</v>
-      </c>
-      <c r="M58" s="2"/>
-      <c r="N58" s="2"/>
+        <v>371</v>
+      </c>
+      <c r="M58" t="s" s="2">
+        <v>372</v>
+      </c>
+      <c r="N58" t="s" s="2">
+        <v>373</v>
+      </c>
       <c r="O58" t="s" s="2">
         <v>39</v>
       </c>
       <c r="P58" s="2"/>
       <c r="Q58" t="s" s="2">
-        <v>39</v>
+        <v>374</v>
       </c>
       <c r="R58" t="s" s="2">
         <v>39</v>
@@ -7783,35 +7744,37 @@
         <v>39</v>
       </c>
       <c r="W58" t="s" s="2">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="X58" t="s" s="2">
-        <v>39</v>
+        <v>375</v>
       </c>
       <c r="Y58" t="s" s="2">
-        <v>39</v>
+        <v>376</v>
       </c>
       <c r="Z58" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AA58" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AB58" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="AB58" t="s" s="2">
+        <v>39</v>
+      </c>
       <c r="AC58" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD58" t="s" s="2">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>78</v>
+        <v>369</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG58" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AH58" t="s" s="2">
         <v>39</v>
@@ -7820,34 +7783,32 @@
         <v>39</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>39</v>
+        <v>191</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>39</v>
+        <v>192</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="59" hidden="true">
+    <row r="59">
       <c r="A59" t="s" s="2">
-        <v>371</v>
-      </c>
-      <c r="B59" t="s" s="2">
-        <v>372</v>
-      </c>
+        <v>377</v>
+      </c>
+      <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
         <v>39</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F59" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G59" t="s" s="2">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="H59" t="s" s="2">
         <v>39</v>
@@ -7856,15 +7817,17 @@
         <v>39</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>373</v>
+        <v>129</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>375</v>
-      </c>
-      <c r="M59" s="2"/>
+        <v>379</v>
+      </c>
+      <c r="M59" t="s" s="2">
+        <v>380</v>
+      </c>
       <c r="N59" s="2"/>
       <c r="O59" t="s" s="2">
         <v>39</v>
@@ -7913,25 +7876,25 @@
         <v>39</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>78</v>
+        <v>377</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG59" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AH59" t="s" s="2">
-        <v>152</v>
+        <v>381</v>
       </c>
       <c r="AI59" t="s" s="2">
-        <v>158</v>
+        <v>39</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>39</v>
+        <v>382</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>39</v>
+        <v>382</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>39</v>
@@ -7939,18 +7902,18 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
-        <v>280</v>
+        <v>39</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" t="s" s="2">
         <v>40</v>
       </c>
       <c r="F60" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="G60" t="s" s="2">
         <v>39</v>
@@ -7962,18 +7925,20 @@
         <v>51</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>71</v>
+        <v>119</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>160</v>
+        <v>384</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>281</v>
+        <v>385</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="N60" s="2"/>
+        <v>386</v>
+      </c>
+      <c r="N60" t="s" s="2">
+        <v>387</v>
+      </c>
       <c r="O60" t="s" s="2">
         <v>39</v>
       </c>
@@ -7997,13 +7962,13 @@
         <v>39</v>
       </c>
       <c r="W60" t="s" s="2">
-        <v>39</v>
+        <v>176</v>
       </c>
       <c r="X60" t="s" s="2">
-        <v>39</v>
+        <v>388</v>
       </c>
       <c r="Y60" t="s" s="2">
-        <v>39</v>
+        <v>389</v>
       </c>
       <c r="Z60" t="s" s="2">
         <v>39</v>
@@ -8021,13 +7986,13 @@
         <v>39</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>282</v>
+        <v>383</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG60" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="AH60" t="s" s="2">
         <v>39</v>
@@ -8036,32 +8001,32 @@
         <v>39</v>
       </c>
       <c r="AJ60" t="s" s="2">
-        <v>143</v>
+        <v>390</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>39</v>
+        <v>193</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>377</v>
+        <v>391</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
-        <v>378</v>
+        <v>39</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F61" t="s" s="2">
         <v>50</v>
       </c>
       <c r="G61" t="s" s="2">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="H61" t="s" s="2">
         <v>39</v>
@@ -8070,19 +8035,19 @@
         <v>39</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>64</v>
+        <v>182</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>379</v>
+        <v>392</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>380</v>
+        <v>393</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>381</v>
+        <v>394</v>
       </c>
       <c r="N61" t="s" s="2">
-        <v>382</v>
+        <v>395</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>39</v>
@@ -8107,13 +8072,13 @@
         <v>39</v>
       </c>
       <c r="W61" t="s" s="2">
-        <v>39</v>
+        <v>188</v>
       </c>
       <c r="X61" t="s" s="2">
-        <v>39</v>
+        <v>396</v>
       </c>
       <c r="Y61" t="s" s="2">
-        <v>39</v>
+        <v>397</v>
       </c>
       <c r="Z61" t="s" s="2">
         <v>39</v>
@@ -8131,7 +8096,7 @@
         <v>39</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>377</v>
+        <v>391</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>40</v>
@@ -8146,10 +8111,10 @@
         <v>39</v>
       </c>
       <c r="AJ61" t="s" s="2">
-        <v>240</v>
+        <v>398</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>241</v>
+        <v>68</v>
       </c>
       <c r="AL61" t="s" s="2">
         <v>39</v>
@@ -8157,7 +8122,7 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>383</v>
+        <v>399</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8180,26 +8145,24 @@
         <v>39</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>182</v>
+        <v>400</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>384</v>
+        <v>401</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>385</v>
+        <v>402</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>386</v>
-      </c>
-      <c r="N62" t="s" s="2">
-        <v>387</v>
-      </c>
+        <v>403</v>
+      </c>
+      <c r="N62" s="2"/>
       <c r="O62" t="s" s="2">
         <v>39</v>
       </c>
       <c r="P62" s="2"/>
       <c r="Q62" t="s" s="2">
-        <v>388</v>
+        <v>39</v>
       </c>
       <c r="R62" t="s" s="2">
         <v>39</v>
@@ -8217,13 +8180,13 @@
         <v>39</v>
       </c>
       <c r="W62" t="s" s="2">
-        <v>109</v>
+        <v>39</v>
       </c>
       <c r="X62" t="s" s="2">
-        <v>389</v>
+        <v>39</v>
       </c>
       <c r="Y62" t="s" s="2">
-        <v>390</v>
+        <v>39</v>
       </c>
       <c r="Z62" t="s" s="2">
         <v>39</v>
@@ -8241,33 +8204,33 @@
         <v>39</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>383</v>
+        <v>399</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG62" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AH62" t="s" s="2">
-        <v>39</v>
+        <v>404</v>
       </c>
       <c r="AI62" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AJ62" t="s" s="2">
-        <v>191</v>
+        <v>405</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>192</v>
+        <v>406</v>
       </c>
       <c r="AL62" t="s" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>391</v>
+        <v>407</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8275,13 +8238,13 @@
       </c>
       <c r="D63" s="2"/>
       <c r="E63" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F63" t="s" s="2">
         <v>50</v>
       </c>
       <c r="G63" t="s" s="2">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="H63" t="s" s="2">
         <v>39</v>
@@ -8290,18 +8253,20 @@
         <v>39</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>129</v>
+        <v>182</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>392</v>
+        <v>408</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>393</v>
+        <v>409</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>394</v>
-      </c>
-      <c r="N63" s="2"/>
+        <v>410</v>
+      </c>
+      <c r="N63" t="s" s="2">
+        <v>411</v>
+      </c>
       <c r="O63" t="s" s="2">
         <v>39</v>
       </c>
@@ -8325,13 +8290,13 @@
         <v>39</v>
       </c>
       <c r="W63" t="s" s="2">
-        <v>39</v>
+        <v>188</v>
       </c>
       <c r="X63" t="s" s="2">
-        <v>39</v>
+        <v>412</v>
       </c>
       <c r="Y63" t="s" s="2">
-        <v>39</v>
+        <v>413</v>
       </c>
       <c r="Z63" t="s" s="2">
         <v>39</v>
@@ -8349,7 +8314,7 @@
         <v>39</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>391</v>
+        <v>407</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>40</v>
@@ -8358,16 +8323,16 @@
         <v>50</v>
       </c>
       <c r="AH63" t="s" s="2">
-        <v>395</v>
+        <v>404</v>
       </c>
       <c r="AI63" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AJ63" t="s" s="2">
-        <v>396</v>
+        <v>414</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>396</v>
+        <v>68</v>
       </c>
       <c r="AL63" t="s" s="2">
         <v>39</v>
@@ -8375,7 +8340,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>397</v>
+        <v>415</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8386,32 +8351,30 @@
         <v>40</v>
       </c>
       <c r="F64" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G64" t="s" s="2">
         <v>39</v>
       </c>
       <c r="H64" t="s" s="2">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="I64" t="s" s="2">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>119</v>
+        <v>39</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>398</v>
+        <v>416</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>399</v>
+        <v>417</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>400</v>
-      </c>
-      <c r="N64" t="s" s="2">
-        <v>401</v>
-      </c>
+        <v>418</v>
+      </c>
+      <c r="N64" s="2"/>
       <c r="O64" t="s" s="2">
         <v>39</v>
       </c>
@@ -8435,13 +8398,13 @@
         <v>39</v>
       </c>
       <c r="W64" t="s" s="2">
-        <v>176</v>
+        <v>39</v>
       </c>
       <c r="X64" t="s" s="2">
-        <v>402</v>
+        <v>39</v>
       </c>
       <c r="Y64" t="s" s="2">
-        <v>403</v>
+        <v>39</v>
       </c>
       <c r="Z64" t="s" s="2">
         <v>39</v>
@@ -8459,468 +8422,32 @@
         <v>39</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>397</v>
+        <v>415</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AG64" t="s" s="2">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AH64" t="s" s="2">
-        <v>39</v>
+        <v>381</v>
       </c>
       <c r="AI64" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AJ64" t="s" s="2">
-        <v>404</v>
+        <v>354</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>68</v>
+        <v>419</v>
       </c>
       <c r="AL64" t="s" s="2">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="65" hidden="true">
-      <c r="A65" t="s" s="2">
-        <v>405</v>
-      </c>
-      <c r="B65" s="2"/>
-      <c r="C65" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D65" s="2"/>
-      <c r="E65" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="F65" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="G65" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="H65" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="I65" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="J65" t="s" s="2">
-        <v>182</v>
-      </c>
-      <c r="K65" t="s" s="2">
-        <v>406</v>
-      </c>
-      <c r="L65" t="s" s="2">
-        <v>407</v>
-      </c>
-      <c r="M65" t="s" s="2">
-        <v>408</v>
-      </c>
-      <c r="N65" t="s" s="2">
-        <v>409</v>
-      </c>
-      <c r="O65" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="P65" s="2"/>
-      <c r="Q65" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="R65" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="S65" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="T65" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="U65" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="V65" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="W65" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="X65" t="s" s="2">
-        <v>410</v>
-      </c>
-      <c r="Y65" t="s" s="2">
-        <v>411</v>
-      </c>
-      <c r="Z65" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA65" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB65" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC65" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD65" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE65" t="s" s="2">
-        <v>405</v>
-      </c>
-      <c r="AF65" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG65" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH65" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI65" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ65" t="s" s="2">
-        <v>412</v>
-      </c>
-      <c r="AK65" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="AL65" t="s" s="2">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="s" s="2">
-        <v>413</v>
-      </c>
-      <c r="B66" s="2"/>
-      <c r="C66" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D66" s="2"/>
-      <c r="E66" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="F66" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="G66" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="H66" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="I66" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="J66" t="s" s="2">
-        <v>414</v>
-      </c>
-      <c r="K66" t="s" s="2">
-        <v>415</v>
-      </c>
-      <c r="L66" t="s" s="2">
-        <v>416</v>
-      </c>
-      <c r="M66" t="s" s="2">
-        <v>417</v>
-      </c>
-      <c r="N66" s="2"/>
-      <c r="O66" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="P66" s="2"/>
-      <c r="Q66" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="R66" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="S66" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="T66" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="U66" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="V66" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="W66" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="X66" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="Y66" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="Z66" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA66" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB66" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC66" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD66" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE66" t="s" s="2">
-        <v>413</v>
-      </c>
-      <c r="AF66" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG66" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AH66" t="s" s="2">
-        <v>418</v>
-      </c>
-      <c r="AI66" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ66" t="s" s="2">
-        <v>419</v>
-      </c>
-      <c r="AK66" t="s" s="2">
-        <v>420</v>
-      </c>
-      <c r="AL66" t="s" s="2">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="67" hidden="true">
-      <c r="A67" t="s" s="2">
-        <v>421</v>
-      </c>
-      <c r="B67" s="2"/>
-      <c r="C67" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D67" s="2"/>
-      <c r="E67" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="F67" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="G67" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="H67" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="I67" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="J67" t="s" s="2">
-        <v>182</v>
-      </c>
-      <c r="K67" t="s" s="2">
-        <v>422</v>
-      </c>
-      <c r="L67" t="s" s="2">
-        <v>423</v>
-      </c>
-      <c r="M67" t="s" s="2">
-        <v>424</v>
-      </c>
-      <c r="N67" t="s" s="2">
-        <v>425</v>
-      </c>
-      <c r="O67" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="P67" s="2"/>
-      <c r="Q67" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="R67" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="S67" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="T67" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="U67" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="V67" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="W67" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="X67" t="s" s="2">
-        <v>426</v>
-      </c>
-      <c r="Y67" t="s" s="2">
-        <v>427</v>
-      </c>
-      <c r="Z67" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA67" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB67" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC67" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD67" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE67" t="s" s="2">
-        <v>421</v>
-      </c>
-      <c r="AF67" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG67" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH67" t="s" s="2">
-        <v>418</v>
-      </c>
-      <c r="AI67" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ67" t="s" s="2">
-        <v>428</v>
-      </c>
-      <c r="AK67" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="AL67" t="s" s="2">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="68" hidden="true">
-      <c r="A68" t="s" s="2">
-        <v>429</v>
-      </c>
-      <c r="B68" s="2"/>
-      <c r="C68" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D68" s="2"/>
-      <c r="E68" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="F68" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="G68" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="H68" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="I68" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="J68" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="K68" t="s" s="2">
-        <v>430</v>
-      </c>
-      <c r="L68" t="s" s="2">
-        <v>431</v>
-      </c>
-      <c r="M68" t="s" s="2">
-        <v>432</v>
-      </c>
-      <c r="N68" s="2"/>
-      <c r="O68" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="P68" s="2"/>
-      <c r="Q68" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="R68" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="S68" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="T68" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="U68" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="V68" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="W68" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="X68" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="Y68" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="Z68" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA68" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB68" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC68" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD68" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE68" t="s" s="2">
-        <v>429</v>
-      </c>
-      <c r="AF68" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG68" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AH68" t="s" s="2">
-        <v>395</v>
-      </c>
-      <c r="AI68" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ68" t="s" s="2">
-        <v>368</v>
-      </c>
-      <c r="AK68" t="s" s="2">
-        <v>433</v>
-      </c>
-      <c r="AL68" t="s" s="2">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AL68">
+  <autoFilter ref="A1:AL64">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -8930,7 +8457,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI67">
+  <conditionalFormatting sqref="A2:AI63">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Build Advance Advance Care Records with latest changes
</commit_message>
<xml_diff>
--- a/output/AdvanceCareRecords/composition-acp-1.xlsx
+++ b/output/AdvanceCareRecords/composition-acp-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$69</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2178" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2347" uniqueCount="436">
   <si>
     <t>Path</t>
   </si>
@@ -153,7 +153,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}inv-dh-cmp-03:If the author is a practitioner, the authoring practitioner role shall be provided {(Composition.author.resolve() is Practitioner) implies Composition.extension('http://hl7.org.au/fhir/StructureDefinition/composition-author-role').exists()}</t>
+dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}inv-dh-cmp-01:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt; 1).exists()}inv-dh-cmp-02:The author shall at least have a reference or an identifier with at least a system and a value {author.reference.exists() or author.identifier.where(system.count() + value.count() &gt; 1).exists()}inv-dh-cmp-04:If and only if the author is a practitioner, the role shall be provided {author.resolve().where($this is Practitioner ).exists() implies extension('http://hl7.org.au/fhir/StructureDefinition/composition-author-role').exists()}inv-dh-cmp-05:If present, an authoring role shall at least have a reference that conforms to PractitionerRole with Practitioner with Mandatory Identifier or an identifier with at least a system and a value {extension('http://hl7.org.au/fhir/StructureDefinition/composition-author-role').exists() implies extension('http://hl7.org.au/fhir/StructureDefinition/composition-author-role').valueReference.reference.resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitionerrole-withpractitionerident-1') or extension('http://hl7.org.au/fhir/StructureDefinition/composition-author-role').valueReference.identifier.where(system.count() + value.count() &gt;1).exists()}inv-dh-cmp-03:The custodian shall at least have a reference or an identifier with at least a system and a value {custodian.reference.exists() or custodian.identifier.where(system.count() + value.count() &gt; 1).exists()}</t>
   </si>
   <si>
     <t>Document[classCode="DOC" and moodCode="EVN" and isNormalAct()]</t>
@@ -206,7 +206,7 @@
     <t>Resource.meta</t>
   </si>
   <si>
-    <t xml:space="preserve">inv-dh-cmp-01:One profile shall be 'http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/composition-acp-1' {profile.where($this='http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/composition-acp-1').exists()}
+    <t xml:space="preserve">inv-dh-cmp-06:One profile shall be 'http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/composition-acp-1' {profile.where($this='http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/composition-acp-1').exists()}
 </t>
   </si>
   <si>
@@ -497,7 +497,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}inv-dh-cmp-04:A practitioner role shall conform to PractitionerRole with Practitioner with Mandatory Identifier {Composition.extension('http://hl7.org.au/fhir/StructureDefinition/composition-author-role').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitioner-ident-1')}</t>
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
     <t>informationRecipient</t>
@@ -511,10 +511,6 @@
   </si>
   <si>
     <t>A recipient who should receive a copy of the composition. A recipient is an entity to whom a copy of the composition is directed at the time of authoring of the composition.</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
     <t>Composition.modifierExtension</t>
@@ -657,7 +653,7 @@
     <t>Composition.subject</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-ident-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-mhr-1)
 </t>
   </si>
   <si>
@@ -738,7 +734,7 @@
     <t>Composition.author</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitioner-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/relatedperson-ident-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitioner-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/relatedperson-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-mhr-1)
 </t>
   </si>
   <si>
@@ -807,7 +803,7 @@
 </t>
   </si>
   <si>
-    <t>Legal attester</t>
+    <t>Legal Attester</t>
   </si>
   <si>
     <t>A participant who has attested to the accuracy of the composition/document.</t>
@@ -820,7 +816,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-inv-com-0:Related party and party shall not coexist {(attester.extension('http://hl7.org.au/fhir/StructureDefinition/attester-related-party').exists() and attester.party.exists()).not()}inv-dh-cmp-02:A legal attester shall have a party or a related party {Composition.attester.party.exists() or Composition.attester.extension('http://hl7.org.au/fhir/StructureDefinition/attester-related-party').exists()}</t>
+inv-com-0:Related party and party shall not coexist {(attester.extension('http://hl7.org.au/fhir/StructureDefinition/attester-related-party').exists() and attester.party.exists()).not()}inv-dh-cmp-08:A legal attester shall have a party or a related party that conforms to RelatedPerson with Mandatory Identifier {party.exists() xor valueReference.reference.resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/relatedperson-ident-1').exists()}inv-dh-cmp-07:If present, a party shall at least have a reference or an identifier with at least a system and a value {party.exists() implies (party.reference.exists() or party.identifier.where(system.count() + value.count() &gt; 1).exists())}</t>
   </si>
   <si>
     <t>.participation[typeCode="AUTHEN"].role[classCode="ASSIGNED"]</t>
@@ -848,10 +844,6 @@
     <t>A related person that attested this composition.</t>
   </si>
   <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}inv-dh-cmp-05:A related party shall conform to RelatedPerson with Mandatory Identifier {Composition.attester.extension('http://hl7.org.au/fhir/StructureDefinition/attester-related-party').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/relatedperson-ident-1')}</t>
-  </si>
-  <si>
     <t>Composition.attester.modifierExtension</t>
   </si>
   <si>
@@ -916,7 +908,7 @@
     <t>Composition.attester.party</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitioner-ident-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitioner-ident-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-mhr-1)
 </t>
   </si>
   <si>
@@ -1189,14 +1181,6 @@
     <t>Provides computable standardized labels to topics within the document.</t>
   </si>
   <si>
-    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
-  &lt;coding&gt;
-    &lt;system value="https://healthterminologies.gov.au/fhir/CodeSystem/nctis-data-components-1"/&gt;
-    &lt;code value="101.16973"/&gt;
-  &lt;/coding&gt;
-&lt;/valueCodeableConcept&gt;</t>
-  </si>
-  <si>
     <t>Classification of a section of a composition/document.</t>
   </si>
   <si>
@@ -1294,6 +1278,66 @@
   </si>
   <si>
     <t>.entry</t>
+  </si>
+  <si>
+    <t>Composition.section.entry.id</t>
+  </si>
+  <si>
+    <t>Composition.section.entry.extension</t>
+  </si>
+  <si>
+    <t>Composition.section.entry.reference</t>
+  </si>
+  <si>
+    <t>Literal reference, Relative, internal or absolute URL</t>
+  </si>
+  <si>
+    <t>A reference to a location at which the other resource is found. The reference may be a relative reference, in which case it is relative to the service base URL, or an absolute URL that resolves to the location where the resource is found. The reference may be version specific or not. If the reference is not to a FHIR RESTful server, then it should be assumed to be version specific. Internal fragment references (start with '#') refer to contained resources.</t>
+  </si>
+  <si>
+    <t>Using absolute URLs provides a stable scalable approach suitable for a cloud/web context, while using relative/logical references provides a flexible approach suitable for use when trading across closed eco-system boundaries.   Absolute URLs do not need to point to a FHIR RESTful server, though this is the preferred approach. If the URL conforms to the structure "/[type]/[id]" then it should be assumed that the reference is to a FHIR RESTful server.</t>
+  </si>
+  <si>
+    <t>Reference.reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ref-1
+</t>
+  </si>
+  <si>
+    <t>Composition.section.entry.identifier</t>
+  </si>
+  <si>
+    <t>Logical reference, when literal reference is not known</t>
+  </si>
+  <si>
+    <t>An identifier for the other resource. This is used when there is no way to reference the other resource directly, either because the entity is not available through a FHIR server, or because there is no way for the author of the resource to convert a known identifier to an actual location. There is no requirement that a Reference.identifier point to something that is actually exposed as a FHIR instance, but it SHALL point to a business concept that would be expected to be exposed as a FHIR instance, and that instance would need to be of a FHIR resource type allowed by the reference.</t>
+  </si>
+  <si>
+    <t>When an identifier is provided in place of a reference, any system processing the reference will only be able to resolve the identifier to a reference if it understands the business context in which the identifier is used. Sometimes this is global (e.g. a national identifier) but often it is not. For this reason, none of the useful mechanisms described for working with references (e.g. chaining, includes) are possible, nor should servers be expected to be able resolve the reference. Servers may accept an identifier based reference untouched, resolve it, and/or reject it - see CapabilityStatement.rest.resource.referencePolicy. 
+When both an identifier and a literal reference are provided, the literal reference is preferred. Applications processing the resource are allowed - but not required - to check that the identifier matches the literal reference
+Applications converting a logical reference to a literal reference may choose to leave the logical reference present, or remove it.</t>
+  </si>
+  <si>
+    <t>Reference.identifier</t>
+  </si>
+  <si>
+    <t>.identifier</t>
+  </si>
+  <si>
+    <t>Composition.section.entry.display</t>
+  </si>
+  <si>
+    <t>Text alternative for the resource</t>
+  </si>
+  <si>
+    <t>Plain text narrative that identifies the resource in addition to the resource reference.</t>
+  </si>
+  <si>
+    <t>This is generally not the same as the Resource.text of the referenced resource.  The purpose is to identify what's being referenced, not to fully describe it.</t>
+  </si>
+  <si>
+    <t>Reference.display</t>
   </si>
   <si>
     <t>Composition.section.emptyReason</t>
@@ -1481,7 +1525,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AL64"/>
+  <dimension ref="A1:AL69"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -3462,7 +3506,7 @@
         <v>152</v>
       </c>
       <c r="AI18" t="s" s="2">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="AJ18" t="s" s="2">
         <v>39</v>
@@ -3476,7 +3520,7 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3502,10 +3546,10 @@
         <v>71</v>
       </c>
       <c r="K19" t="s" s="2">
+        <v>159</v>
+      </c>
+      <c r="L19" t="s" s="2">
         <v>160</v>
-      </c>
-      <c r="L19" t="s" s="2">
-        <v>161</v>
       </c>
       <c r="M19" t="s" s="2">
         <v>74</v>
@@ -3558,7 +3602,7 @@
         <v>39</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>40</v>
@@ -3584,7 +3628,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3607,16 +3651,16 @@
         <v>51</v>
       </c>
       <c r="J20" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="K20" t="s" s="2">
         <v>164</v>
       </c>
-      <c r="K20" t="s" s="2">
+      <c r="L20" t="s" s="2">
         <v>165</v>
       </c>
-      <c r="L20" t="s" s="2">
+      <c r="M20" t="s" s="2">
         <v>166</v>
-      </c>
-      <c r="M20" t="s" s="2">
-        <v>167</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
@@ -3666,7 +3710,7 @@
         <v>39</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>40</v>
@@ -3681,18 +3725,18 @@
         <v>39</v>
       </c>
       <c r="AJ20" t="s" s="2">
+        <v>167</v>
+      </c>
+      <c r="AK20" t="s" s="2">
         <v>168</v>
       </c>
-      <c r="AK20" t="s" s="2">
+      <c r="AL20" t="s" s="2">
         <v>169</v>
-      </c>
-      <c r="AL20" t="s" s="2">
-        <v>170</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3718,16 +3762,16 @@
         <v>119</v>
       </c>
       <c r="K21" t="s" s="2">
+        <v>171</v>
+      </c>
+      <c r="L21" t="s" s="2">
         <v>172</v>
       </c>
-      <c r="L21" t="s" s="2">
+      <c r="M21" t="s" s="2">
         <v>173</v>
       </c>
-      <c r="M21" t="s" s="2">
+      <c r="N21" t="s" s="2">
         <v>174</v>
-      </c>
-      <c r="N21" t="s" s="2">
-        <v>175</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>39</v>
@@ -3752,57 +3796,57 @@
         <v>39</v>
       </c>
       <c r="W21" t="s" s="2">
+        <v>175</v>
+      </c>
+      <c r="X21" t="s" s="2">
         <v>176</v>
       </c>
-      <c r="X21" t="s" s="2">
+      <c r="Y21" t="s" s="2">
         <v>177</v>
       </c>
-      <c r="Y21" t="s" s="2">
+      <c r="Z21" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA21" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB21" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC21" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD21" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE21" t="s" s="2">
+        <v>170</v>
+      </c>
+      <c r="AF21" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AG21" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH21" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI21" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ21" t="s" s="2">
         <v>178</v>
-      </c>
-      <c r="Z21" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA21" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB21" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC21" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD21" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE21" t="s" s="2">
-        <v>171</v>
-      </c>
-      <c r="AF21" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AG21" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH21" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI21" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ21" t="s" s="2">
-        <v>179</v>
       </c>
       <c r="AK21" t="s" s="2">
         <v>68</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3825,94 +3869,94 @@
         <v>51</v>
       </c>
       <c r="J22" t="s" s="2">
+        <v>181</v>
+      </c>
+      <c r="K22" t="s" s="2">
         <v>182</v>
       </c>
-      <c r="K22" t="s" s="2">
+      <c r="L22" t="s" s="2">
         <v>183</v>
       </c>
-      <c r="L22" t="s" s="2">
+      <c r="M22" t="s" s="2">
         <v>184</v>
       </c>
-      <c r="M22" t="s" s="2">
+      <c r="N22" t="s" s="2">
         <v>185</v>
-      </c>
-      <c r="N22" t="s" s="2">
-        <v>186</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>39</v>
       </c>
       <c r="P22" s="2"/>
       <c r="Q22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R22" t="s" s="2">
+        <v>186</v>
+      </c>
+      <c r="S22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W22" t="s" s="2">
         <v>187</v>
       </c>
-      <c r="R22" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="S22" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="T22" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="U22" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="V22" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="W22" t="s" s="2">
+      <c r="X22" t="s" s="2">
         <v>188</v>
       </c>
-      <c r="X22" t="s" s="2">
+      <c r="Y22" t="s" s="2">
         <v>189</v>
       </c>
-      <c r="Y22" t="s" s="2">
+      <c r="Z22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE22" t="s" s="2">
+        <v>180</v>
+      </c>
+      <c r="AF22" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AG22" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI22" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ22" t="s" s="2">
         <v>190</v>
       </c>
-      <c r="Z22" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA22" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB22" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC22" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD22" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE22" t="s" s="2">
-        <v>181</v>
-      </c>
-      <c r="AF22" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AG22" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH22" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI22" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ22" t="s" s="2">
+      <c r="AK22" t="s" s="2">
         <v>191</v>
       </c>
-      <c r="AK22" t="s" s="2">
+      <c r="AL22" t="s" s="2">
         <v>192</v>
-      </c>
-      <c r="AL22" t="s" s="2">
-        <v>193</v>
       </c>
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3935,19 +3979,19 @@
         <v>51</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K23" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="L23" t="s" s="2">
         <v>195</v>
       </c>
-      <c r="L23" t="s" s="2">
+      <c r="M23" t="s" s="2">
         <v>196</v>
       </c>
-      <c r="M23" t="s" s="2">
+      <c r="N23" t="s" s="2">
         <v>197</v>
-      </c>
-      <c r="N23" t="s" s="2">
-        <v>198</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>39</v>
@@ -3975,54 +4019,54 @@
         <v>109</v>
       </c>
       <c r="X23" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="Y23" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="Y23" t="s" s="2">
+      <c r="Z23" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA23" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB23" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC23" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD23" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE23" t="s" s="2">
+        <v>193</v>
+      </c>
+      <c r="AF23" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG23" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH23" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI23" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ23" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="Z23" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA23" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB23" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC23" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD23" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE23" t="s" s="2">
-        <v>194</v>
-      </c>
-      <c r="AF23" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG23" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH23" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI23" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ23" t="s" s="2">
-        <v>201</v>
       </c>
       <c r="AK23" t="s" s="2">
         <v>68</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4045,19 +4089,19 @@
         <v>51</v>
       </c>
       <c r="J24" t="s" s="2">
+        <v>202</v>
+      </c>
+      <c r="K24" t="s" s="2">
         <v>203</v>
       </c>
-      <c r="K24" t="s" s="2">
+      <c r="L24" t="s" s="2">
         <v>204</v>
       </c>
-      <c r="L24" t="s" s="2">
+      <c r="M24" t="s" s="2">
         <v>205</v>
       </c>
-      <c r="M24" t="s" s="2">
+      <c r="N24" t="s" s="2">
         <v>206</v>
-      </c>
-      <c r="N24" t="s" s="2">
-        <v>207</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>39</v>
@@ -4106,7 +4150,7 @@
         <v>39</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>50</v>
@@ -4121,18 +4165,18 @@
         <v>39</v>
       </c>
       <c r="AJ24" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="AK24" t="s" s="2">
         <v>208</v>
       </c>
-      <c r="AK24" t="s" s="2">
+      <c r="AL24" t="s" s="2">
         <v>209</v>
-      </c>
-      <c r="AL24" t="s" s="2">
-        <v>210</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4155,17 +4199,17 @@
         <v>51</v>
       </c>
       <c r="J25" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="K25" t="s" s="2">
         <v>212</v>
       </c>
-      <c r="K25" t="s" s="2">
+      <c r="L25" t="s" s="2">
         <v>213</v>
-      </c>
-      <c r="L25" t="s" s="2">
-        <v>214</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" t="s" s="2">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>39</v>
@@ -4214,7 +4258,7 @@
         <v>39</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>40</v>
@@ -4229,18 +4273,18 @@
         <v>39</v>
       </c>
       <c r="AJ25" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="AK25" t="s" s="2">
         <v>216</v>
       </c>
-      <c r="AK25" t="s" s="2">
+      <c r="AL25" t="s" s="2">
         <v>217</v>
-      </c>
-      <c r="AL25" t="s" s="2">
-        <v>218</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4263,19 +4307,19 @@
         <v>51</v>
       </c>
       <c r="J26" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="K26" t="s" s="2">
         <v>220</v>
       </c>
-      <c r="K26" t="s" s="2">
+      <c r="L26" t="s" s="2">
         <v>221</v>
       </c>
-      <c r="L26" t="s" s="2">
+      <c r="M26" t="s" s="2">
         <v>222</v>
       </c>
-      <c r="M26" t="s" s="2">
+      <c r="N26" t="s" s="2">
         <v>223</v>
-      </c>
-      <c r="N26" t="s" s="2">
-        <v>224</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>39</v>
@@ -4324,7 +4368,7 @@
         <v>39</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>50</v>
@@ -4339,18 +4383,18 @@
         <v>39</v>
       </c>
       <c r="AJ26" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="AK26" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="AK26" t="s" s="2">
+      <c r="AL26" t="s" s="2">
         <v>226</v>
-      </c>
-      <c r="AL26" t="s" s="2">
-        <v>227</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4373,17 +4417,17 @@
         <v>51</v>
       </c>
       <c r="J27" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="K27" t="s" s="2">
         <v>229</v>
       </c>
-      <c r="K27" t="s" s="2">
+      <c r="L27" t="s" s="2">
         <v>230</v>
-      </c>
-      <c r="L27" t="s" s="2">
-        <v>231</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" t="s" s="2">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>39</v>
@@ -4432,7 +4476,7 @@
         <v>39</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>50</v>
@@ -4447,18 +4491,18 @@
         <v>39</v>
       </c>
       <c r="AJ27" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="AK27" t="s" s="2">
         <v>233</v>
       </c>
-      <c r="AK27" t="s" s="2">
+      <c r="AL27" t="s" s="2">
         <v>234</v>
-      </c>
-      <c r="AL27" t="s" s="2">
-        <v>235</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4484,13 +4528,13 @@
         <v>64</v>
       </c>
       <c r="K28" t="s" s="2">
+        <v>236</v>
+      </c>
+      <c r="L28" t="s" s="2">
         <v>237</v>
       </c>
-      <c r="L28" t="s" s="2">
+      <c r="M28" t="s" s="2">
         <v>238</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>239</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
@@ -4540,7 +4584,7 @@
         <v>39</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>50</v>
@@ -4555,10 +4599,10 @@
         <v>39</v>
       </c>
       <c r="AJ28" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="AK28" t="s" s="2">
         <v>240</v>
-      </c>
-      <c r="AK28" t="s" s="2">
-        <v>241</v>
       </c>
       <c r="AL28" t="s" s="2">
         <v>39</v>
@@ -4566,7 +4610,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4592,13 +4636,13 @@
         <v>119</v>
       </c>
       <c r="K29" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="L29" t="s" s="2">
         <v>243</v>
       </c>
-      <c r="L29" t="s" s="2">
+      <c r="M29" t="s" s="2">
         <v>244</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>245</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
@@ -4624,49 +4668,49 @@
         <v>39</v>
       </c>
       <c r="W29" t="s" s="2">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="X29" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="Y29" t="s" s="2">
         <v>246</v>
       </c>
-      <c r="Y29" t="s" s="2">
+      <c r="Z29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE29" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="AF29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG29" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ29" t="s" s="2">
         <v>247</v>
       </c>
-      <c r="Z29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE29" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="AF29" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG29" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ29" t="s" s="2">
-        <v>248</v>
-      </c>
       <c r="AK29" t="s" s="2">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="AL29" t="s" s="2">
         <v>39</v>
@@ -4674,7 +4718,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4697,19 +4741,19 @@
         <v>51</v>
       </c>
       <c r="J30" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="K30" t="s" s="2">
         <v>250</v>
       </c>
-      <c r="K30" t="s" s="2">
+      <c r="L30" t="s" s="2">
         <v>251</v>
       </c>
-      <c r="L30" t="s" s="2">
+      <c r="M30" t="s" s="2">
         <v>252</v>
       </c>
-      <c r="M30" t="s" s="2">
+      <c r="N30" t="s" s="2">
         <v>253</v>
-      </c>
-      <c r="N30" t="s" s="2">
-        <v>254</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>39</v>
@@ -4758,7 +4802,7 @@
         <v>39</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>40</v>
@@ -4770,13 +4814,13 @@
         <v>39</v>
       </c>
       <c r="AI30" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="AJ30" t="s" s="2">
         <v>255</v>
       </c>
-      <c r="AJ30" t="s" s="2">
+      <c r="AK30" t="s" s="2">
         <v>256</v>
-      </c>
-      <c r="AK30" t="s" s="2">
-        <v>257</v>
       </c>
       <c r="AL30" t="s" s="2">
         <v>39</v>
@@ -4784,7 +4828,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4890,7 +4934,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4994,10 +5038,10 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
+        <v>258</v>
+      </c>
+      <c r="B33" t="s" s="2">
         <v>259</v>
-      </c>
-      <c r="B33" t="s" s="2">
-        <v>260</v>
       </c>
       <c r="C33" t="s" s="2">
         <v>39</v>
@@ -5019,13 +5063,13 @@
         <v>39</v>
       </c>
       <c r="J33" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="K33" t="s" s="2">
         <v>261</v>
       </c>
-      <c r="K33" t="s" s="2">
+      <c r="L33" t="s" s="2">
         <v>262</v>
-      </c>
-      <c r="L33" t="s" s="2">
-        <v>263</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -5088,7 +5132,7 @@
         <v>152</v>
       </c>
       <c r="AI33" t="s" s="2">
-        <v>264</v>
+        <v>153</v>
       </c>
       <c r="AJ33" t="s" s="2">
         <v>39</v>
@@ -5102,11 +5146,11 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
@@ -5128,10 +5172,10 @@
         <v>71</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="M34" t="s" s="2">
         <v>74</v>
@@ -5184,7 +5228,7 @@
         <v>39</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>40</v>
@@ -5210,7 +5254,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5236,48 +5280,48 @@
         <v>119</v>
       </c>
       <c r="K35" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="L35" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="M35" t="s" s="2">
         <v>270</v>
       </c>
-      <c r="L35" t="s" s="2">
+      <c r="N35" t="s" s="2">
         <v>271</v>
-      </c>
-      <c r="M35" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>273</v>
       </c>
       <c r="O35" t="s" s="2">
         <v>39</v>
       </c>
       <c r="P35" s="2"/>
       <c r="Q35" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="R35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W35" t="s" s="2">
+        <v>175</v>
+      </c>
+      <c r="X35" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="Y35" t="s" s="2">
         <v>274</v>
       </c>
-      <c r="R35" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="S35" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="T35" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="U35" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="V35" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="W35" t="s" s="2">
-        <v>176</v>
-      </c>
-      <c r="X35" t="s" s="2">
-        <v>275</v>
-      </c>
-      <c r="Y35" t="s" s="2">
-        <v>276</v>
-      </c>
       <c r="Z35" t="s" s="2">
         <v>39</v>
       </c>
@@ -5294,7 +5338,7 @@
         <v>39</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>50</v>
@@ -5309,10 +5353,10 @@
         <v>39</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="AL35" t="s" s="2">
         <v>39</v>
@@ -5320,7 +5364,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5343,17 +5387,17 @@
         <v>51</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" t="s" s="2">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="O36" t="s" s="2">
         <v>39</v>
@@ -5402,7 +5446,7 @@
         <v>39</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>40</v>
@@ -5417,10 +5461,10 @@
         <v>39</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="AL36" t="s" s="2">
         <v>39</v>
@@ -5428,7 +5472,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5451,17 +5495,17 @@
         <v>51</v>
       </c>
       <c r="J37" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="K37" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="L37" t="s" s="2">
         <v>286</v>
-      </c>
-      <c r="K37" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="L37" t="s" s="2">
-        <v>288</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" t="s" s="2">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>39</v>
@@ -5510,7 +5554,7 @@
         <v>39</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>40</v>
@@ -5525,18 +5569,18 @@
         <v>39</v>
       </c>
       <c r="AJ37" t="s" s="2">
+        <v>288</v>
+      </c>
+      <c r="AK37" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="AL37" t="s" s="2">
         <v>290</v>
-      </c>
-      <c r="AK37" t="s" s="2">
-        <v>291</v>
-      </c>
-      <c r="AL37" t="s" s="2">
-        <v>292</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5559,19 +5603,19 @@
         <v>51</v>
       </c>
       <c r="J38" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="K38" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="L38" t="s" s="2">
         <v>294</v>
       </c>
-      <c r="K38" t="s" s="2">
+      <c r="M38" t="s" s="2">
         <v>295</v>
       </c>
-      <c r="L38" t="s" s="2">
+      <c r="N38" t="s" s="2">
         <v>296</v>
-      </c>
-      <c r="M38" t="s" s="2">
-        <v>297</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>298</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>39</v>
@@ -5620,7 +5664,7 @@
         <v>39</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>40</v>
@@ -5635,10 +5679,10 @@
         <v>39</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="AL38" t="s" s="2">
         <v>39</v>
@@ -5646,7 +5690,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5669,16 +5713,16 @@
         <v>51</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K39" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="L39" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="M39" t="s" s="2">
         <v>302</v>
-      </c>
-      <c r="L39" t="s" s="2">
-        <v>303</v>
-      </c>
-      <c r="M39" t="s" s="2">
-        <v>304</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
@@ -5728,7 +5772,7 @@
         <v>39</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>40</v>
@@ -5740,13 +5784,13 @@
         <v>39</v>
       </c>
       <c r="AI39" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="AJ39" t="s" s="2">
+        <v>304</v>
+      </c>
+      <c r="AK39" t="s" s="2">
         <v>305</v>
-      </c>
-      <c r="AJ39" t="s" s="2">
-        <v>306</v>
-      </c>
-      <c r="AK39" t="s" s="2">
-        <v>307</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>39</v>
@@ -5754,7 +5798,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5860,7 +5904,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5968,11 +6012,11 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" t="s" s="2">
@@ -5994,10 +6038,10 @@
         <v>71</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="M42" t="s" s="2">
         <v>74</v>
@@ -6050,7 +6094,7 @@
         <v>39</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>40</v>
@@ -6076,7 +6120,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6102,13 +6146,13 @@
         <v>119</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="L43" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="M43" t="s" s="2">
         <v>312</v>
-      </c>
-      <c r="L43" t="s" s="2">
-        <v>313</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>314</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
@@ -6134,49 +6178,49 @@
         <v>39</v>
       </c>
       <c r="W43" t="s" s="2">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="X43" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="Y43" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="Z43" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA43" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB43" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC43" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD43" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE43" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="AF43" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AG43" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH43" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI43" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ43" t="s" s="2">
         <v>315</v>
       </c>
-      <c r="Y43" t="s" s="2">
+      <c r="AK43" t="s" s="2">
         <v>316</v>
-      </c>
-      <c r="Z43" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA43" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB43" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC43" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD43" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE43" t="s" s="2">
-        <v>311</v>
-      </c>
-      <c r="AF43" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AG43" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH43" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI43" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ43" t="s" s="2">
-        <v>317</v>
-      </c>
-      <c r="AK43" t="s" s="2">
-        <v>318</v>
       </c>
       <c r="AL43" t="s" s="2">
         <v>39</v>
@@ -6184,7 +6228,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6207,13 +6251,13 @@
         <v>51</v>
       </c>
       <c r="J44" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="K44" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="L44" t="s" s="2">
         <v>320</v>
-      </c>
-      <c r="K44" t="s" s="2">
-        <v>321</v>
-      </c>
-      <c r="L44" t="s" s="2">
-        <v>322</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -6264,7 +6308,7 @@
         <v>39</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>50</v>
@@ -6279,10 +6323,10 @@
         <v>39</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>39</v>
@@ -6290,7 +6334,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6313,19 +6357,19 @@
         <v>51</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K45" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="L45" t="s" s="2">
+        <v>325</v>
+      </c>
+      <c r="M45" t="s" s="2">
         <v>326</v>
       </c>
-      <c r="L45" t="s" s="2">
+      <c r="N45" t="s" s="2">
         <v>327</v>
-      </c>
-      <c r="M45" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="N45" t="s" s="2">
-        <v>329</v>
       </c>
       <c r="O45" t="s" s="2">
         <v>39</v>
@@ -6374,7 +6418,7 @@
         <v>39</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>40</v>
@@ -6386,13 +6430,13 @@
         <v>39</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="AL45" t="s" s="2">
         <v>39</v>
@@ -6400,7 +6444,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6506,7 +6550,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6614,11 +6658,11 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
@@ -6640,10 +6684,10 @@
         <v>71</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="M48" t="s" s="2">
         <v>74</v>
@@ -6696,7 +6740,7 @@
         <v>39</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>40</v>
@@ -6722,7 +6766,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6745,16 +6789,16 @@
         <v>51</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K49" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="L49" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="M49" t="s" s="2">
         <v>336</v>
-      </c>
-      <c r="L49" t="s" s="2">
-        <v>337</v>
-      </c>
-      <c r="M49" t="s" s="2">
-        <v>338</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" t="s" s="2">
@@ -6783,10 +6827,10 @@
         <v>109</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="Z49" t="s" s="2">
         <v>39</v>
@@ -6804,7 +6848,7 @@
         <v>39</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>40</v>
@@ -6819,10 +6863,10 @@
         <v>39</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>39</v>
@@ -6830,7 +6874,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6853,13 +6897,13 @@
         <v>51</v>
       </c>
       <c r="J50" t="s" s="2">
+        <v>340</v>
+      </c>
+      <c r="K50" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="L50" t="s" s="2">
         <v>342</v>
-      </c>
-      <c r="K50" t="s" s="2">
-        <v>343</v>
-      </c>
-      <c r="L50" t="s" s="2">
-        <v>344</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -6910,7 +6954,7 @@
         <v>39</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>40</v>
@@ -6925,10 +6969,10 @@
         <v>39</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>39</v>
@@ -6936,7 +6980,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -6959,13 +7003,13 @@
         <v>51</v>
       </c>
       <c r="J51" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="K51" t="s" s="2">
+        <v>345</v>
+      </c>
+      <c r="L51" t="s" s="2">
         <v>346</v>
-      </c>
-      <c r="K51" t="s" s="2">
-        <v>347</v>
-      </c>
-      <c r="L51" t="s" s="2">
-        <v>348</v>
       </c>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -7016,7 +7060,7 @@
         <v>39</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>40</v>
@@ -7031,7 +7075,7 @@
         <v>39</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="AK51" t="s" s="2">
         <v>68</v>
@@ -7042,7 +7086,7 @@
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7065,13 +7109,13 @@
         <v>39</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
@@ -7122,7 +7166,7 @@
         <v>39</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>40</v>
@@ -7134,13 +7178,13 @@
         <v>39</v>
       </c>
       <c r="AI52" t="s" s="2">
+        <v>351</v>
+      </c>
+      <c r="AJ52" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="AK52" t="s" s="2">
         <v>353</v>
-      </c>
-      <c r="AJ52" t="s" s="2">
-        <v>354</v>
-      </c>
-      <c r="AK52" t="s" s="2">
-        <v>355</v>
       </c>
       <c r="AL52" t="s" s="2">
         <v>39</v>
@@ -7148,7 +7192,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7254,7 +7298,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7358,10 +7402,10 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C55" t="s" s="2">
         <v>39</v>
@@ -7383,13 +7427,13 @@
         <v>39</v>
       </c>
       <c r="J55" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="K55" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="L55" t="s" s="2">
         <v>359</v>
-      </c>
-      <c r="K55" t="s" s="2">
-        <v>360</v>
-      </c>
-      <c r="L55" t="s" s="2">
-        <v>361</v>
       </c>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -7452,7 +7496,7 @@
         <v>152</v>
       </c>
       <c r="AI55" t="s" s="2">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="AJ55" t="s" s="2">
         <v>39</v>
@@ -7466,11 +7510,11 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" t="s" s="2">
@@ -7492,10 +7536,10 @@
         <v>71</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="M56" t="s" s="2">
         <v>74</v>
@@ -7548,7 +7592,7 @@
         <v>39</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>40</v>
@@ -7574,11 +7618,11 @@
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" t="s" s="2">
@@ -7600,16 +7644,16 @@
         <v>64</v>
       </c>
       <c r="K57" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="L57" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="M57" t="s" s="2">
         <v>365</v>
       </c>
-      <c r="L57" t="s" s="2">
+      <c r="N57" t="s" s="2">
         <v>366</v>
-      </c>
-      <c r="M57" t="s" s="2">
-        <v>367</v>
-      </c>
-      <c r="N57" t="s" s="2">
-        <v>368</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>39</v>
@@ -7658,7 +7702,7 @@
         <v>39</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>40</v>
@@ -7673,10 +7717,10 @@
         <v>39</v>
       </c>
       <c r="AJ57" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="AK57" t="s" s="2">
         <v>240</v>
-      </c>
-      <c r="AK57" t="s" s="2">
-        <v>241</v>
       </c>
       <c r="AL57" t="s" s="2">
         <v>39</v>
@@ -7684,7 +7728,7 @@
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7707,29 +7751,29 @@
         <v>39</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K58" t="s" s="2">
+        <v>368</v>
+      </c>
+      <c r="L58" t="s" s="2">
+        <v>369</v>
+      </c>
+      <c r="M58" t="s" s="2">
         <v>370</v>
       </c>
-      <c r="L58" t="s" s="2">
+      <c r="N58" t="s" s="2">
         <v>371</v>
-      </c>
-      <c r="M58" t="s" s="2">
-        <v>372</v>
-      </c>
-      <c r="N58" t="s" s="2">
-        <v>373</v>
       </c>
       <c r="O58" t="s" s="2">
         <v>39</v>
       </c>
       <c r="P58" s="2"/>
       <c r="Q58" t="s" s="2">
-        <v>374</v>
+        <v>39</v>
       </c>
       <c r="R58" t="s" s="2">
-        <v>39</v>
+        <v>186</v>
       </c>
       <c r="S58" t="s" s="2">
         <v>39</v>
@@ -7747,10 +7791,10 @@
         <v>109</v>
       </c>
       <c r="X58" t="s" s="2">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="Y58" t="s" s="2">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="Z58" t="s" s="2">
         <v>39</v>
@@ -7768,7 +7812,7 @@
         <v>39</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>40</v>
@@ -7783,10 +7827,10 @@
         <v>39</v>
       </c>
       <c r="AJ58" t="s" s="2">
+        <v>190</v>
+      </c>
+      <c r="AK58" t="s" s="2">
         <v>191</v>
-      </c>
-      <c r="AK58" t="s" s="2">
-        <v>192</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>39</v>
@@ -7794,7 +7838,7 @@
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -7820,13 +7864,13 @@
         <v>129</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" t="s" s="2">
@@ -7876,7 +7920,7 @@
         <v>39</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>40</v>
@@ -7885,16 +7929,16 @@
         <v>50</v>
       </c>
       <c r="AH59" t="s" s="2">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="AI59" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>39</v>
@@ -7902,7 +7946,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -7928,16 +7972,16 @@
         <v>119</v>
       </c>
       <c r="K60" t="s" s="2">
+        <v>381</v>
+      </c>
+      <c r="L60" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="M60" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="N60" t="s" s="2">
         <v>384</v>
-      </c>
-      <c r="L60" t="s" s="2">
-        <v>385</v>
-      </c>
-      <c r="M60" t="s" s="2">
-        <v>386</v>
-      </c>
-      <c r="N60" t="s" s="2">
-        <v>387</v>
       </c>
       <c r="O60" t="s" s="2">
         <v>39</v>
@@ -7962,13 +8006,13 @@
         <v>39</v>
       </c>
       <c r="W60" t="s" s="2">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="X60" t="s" s="2">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="Y60" t="s" s="2">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="Z60" t="s" s="2">
         <v>39</v>
@@ -7986,7 +8030,7 @@
         <v>39</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>40</v>
@@ -8001,18 +8045,18 @@
         <v>39</v>
       </c>
       <c r="AJ60" t="s" s="2">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="AK60" t="s" s="2">
         <v>68</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8035,19 +8079,19 @@
         <v>39</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K61" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="L61" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="M61" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="N61" t="s" s="2">
         <v>392</v>
-      </c>
-      <c r="L61" t="s" s="2">
-        <v>393</v>
-      </c>
-      <c r="M61" t="s" s="2">
-        <v>394</v>
-      </c>
-      <c r="N61" t="s" s="2">
-        <v>395</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>39</v>
@@ -8072,13 +8116,13 @@
         <v>39</v>
       </c>
       <c r="W61" t="s" s="2">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="X61" t="s" s="2">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="Y61" t="s" s="2">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="Z61" t="s" s="2">
         <v>39</v>
@@ -8096,7 +8140,7 @@
         <v>39</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>40</v>
@@ -8111,7 +8155,7 @@
         <v>39</v>
       </c>
       <c r="AJ61" t="s" s="2">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="AK61" t="s" s="2">
         <v>68</v>
@@ -8122,7 +8166,7 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8145,16 +8189,16 @@
         <v>39</v>
       </c>
       <c r="J62" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="K62" t="s" s="2">
+        <v>398</v>
+      </c>
+      <c r="L62" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="M62" t="s" s="2">
         <v>400</v>
-      </c>
-      <c r="K62" t="s" s="2">
-        <v>401</v>
-      </c>
-      <c r="L62" t="s" s="2">
-        <v>402</v>
-      </c>
-      <c r="M62" t="s" s="2">
-        <v>403</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" t="s" s="2">
@@ -8204,7 +8248,7 @@
         <v>39</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>40</v>
@@ -8213,16 +8257,16 @@
         <v>41</v>
       </c>
       <c r="AH62" t="s" s="2">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="AI62" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AJ62" t="s" s="2">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="AL62" t="s" s="2">
         <v>39</v>
@@ -8230,7 +8274,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8253,20 +8297,16 @@
         <v>39</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>182</v>
+        <v>64</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>408</v>
+        <v>65</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>409</v>
-      </c>
-      <c r="M63" t="s" s="2">
-        <v>410</v>
-      </c>
-      <c r="N63" t="s" s="2">
-        <v>411</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="M63" s="2"/>
+      <c r="N63" s="2"/>
       <c r="O63" t="s" s="2">
         <v>39</v>
       </c>
@@ -8290,13 +8330,13 @@
         <v>39</v>
       </c>
       <c r="W63" t="s" s="2">
-        <v>188</v>
+        <v>39</v>
       </c>
       <c r="X63" t="s" s="2">
-        <v>412</v>
+        <v>39</v>
       </c>
       <c r="Y63" t="s" s="2">
-        <v>413</v>
+        <v>39</v>
       </c>
       <c r="Z63" t="s" s="2">
         <v>39</v>
@@ -8314,7 +8354,7 @@
         <v>39</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>407</v>
+        <v>67</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>40</v>
@@ -8323,16 +8363,16 @@
         <v>50</v>
       </c>
       <c r="AH63" t="s" s="2">
-        <v>404</v>
+        <v>39</v>
       </c>
       <c r="AI63" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AJ63" t="s" s="2">
-        <v>414</v>
+        <v>68</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="AL63" t="s" s="2">
         <v>39</v>
@@ -8340,11 +8380,11 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" t="s" s="2">
@@ -8363,16 +8403,16 @@
         <v>39</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>416</v>
+        <v>72</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>417</v>
+        <v>73</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>418</v>
+        <v>74</v>
       </c>
       <c r="N64" s="2"/>
       <c r="O64" t="s" s="2">
@@ -8410,19 +8450,19 @@
         <v>39</v>
       </c>
       <c r="AA64" t="s" s="2">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="AB64" t="s" s="2">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="AC64" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD64" t="s" s="2">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>415</v>
+        <v>78</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>40</v>
@@ -8431,23 +8471,565 @@
         <v>41</v>
       </c>
       <c r="AH64" t="s" s="2">
-        <v>381</v>
+        <v>39</v>
       </c>
       <c r="AI64" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AJ64" t="s" s="2">
-        <v>354</v>
+        <v>68</v>
       </c>
       <c r="AK64" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL64" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="65" hidden="true">
+      <c r="A65" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="B65" s="2"/>
+      <c r="C65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="F65" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I65" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="J65" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="K65" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="L65" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="M65" t="s" s="2">
+        <v>409</v>
+      </c>
+      <c r="N65" s="2"/>
+      <c r="O65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P65" s="2"/>
+      <c r="Q65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE65" t="s" s="2">
+        <v>410</v>
+      </c>
+      <c r="AF65" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG65" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH65" t="s" s="2">
+        <v>411</v>
+      </c>
+      <c r="AI65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ65" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="AK65" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL65" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="66" hidden="true">
+      <c r="A66" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="B66" s="2"/>
+      <c r="C66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F66" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I66" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="J66" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="K66" t="s" s="2">
+        <v>413</v>
+      </c>
+      <c r="L66" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="M66" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="N66" s="2"/>
+      <c r="O66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P66" s="2"/>
+      <c r="Q66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE66" t="s" s="2">
+        <v>416</v>
+      </c>
+      <c r="AF66" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG66" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ66" t="s" s="2">
+        <v>417</v>
+      </c>
+      <c r="AK66" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL66" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" hidden="true">
+      <c r="A67" t="s" s="2">
+        <v>418</v>
+      </c>
+      <c r="B67" s="2"/>
+      <c r="C67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F67" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I67" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="J67" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="K67" t="s" s="2">
         <v>419</v>
       </c>
-      <c r="AL64" t="s" s="2">
+      <c r="L67" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="M67" t="s" s="2">
+        <v>421</v>
+      </c>
+      <c r="N67" s="2"/>
+      <c r="O67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P67" s="2"/>
+      <c r="Q67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE67" t="s" s="2">
+        <v>422</v>
+      </c>
+      <c r="AF67" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG67" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ67" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="AK67" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL67" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="68" hidden="true">
+      <c r="A68" t="s" s="2">
+        <v>423</v>
+      </c>
+      <c r="B68" s="2"/>
+      <c r="C68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F68" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="G68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J68" t="s" s="2">
+        <v>181</v>
+      </c>
+      <c r="K68" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="L68" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="M68" t="s" s="2">
+        <v>426</v>
+      </c>
+      <c r="N68" t="s" s="2">
+        <v>427</v>
+      </c>
+      <c r="O68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P68" s="2"/>
+      <c r="Q68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W68" t="s" s="2">
+        <v>187</v>
+      </c>
+      <c r="X68" t="s" s="2">
+        <v>428</v>
+      </c>
+      <c r="Y68" t="s" s="2">
+        <v>429</v>
+      </c>
+      <c r="Z68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE68" t="s" s="2">
+        <v>423</v>
+      </c>
+      <c r="AF68" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG68" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH68" t="s" s="2">
+        <v>401</v>
+      </c>
+      <c r="AI68" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ68" t="s" s="2">
+        <v>430</v>
+      </c>
+      <c r="AK68" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="AL68" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="69" hidden="true">
+      <c r="A69" t="s" s="2">
+        <v>431</v>
+      </c>
+      <c r="B69" s="2"/>
+      <c r="C69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D69" s="2"/>
+      <c r="E69" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F69" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="G69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="J69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="K69" t="s" s="2">
+        <v>432</v>
+      </c>
+      <c r="L69" t="s" s="2">
+        <v>433</v>
+      </c>
+      <c r="M69" t="s" s="2">
+        <v>434</v>
+      </c>
+      <c r="N69" s="2"/>
+      <c r="O69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P69" s="2"/>
+      <c r="Q69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE69" t="s" s="2">
+        <v>431</v>
+      </c>
+      <c r="AF69" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG69" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AH69" t="s" s="2">
+        <v>378</v>
+      </c>
+      <c r="AI69" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ69" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="AK69" t="s" s="2">
+        <v>435</v>
+      </c>
+      <c r="AL69" t="s" s="2">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AL64">
+  <autoFilter ref="A1:AL69">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -8457,7 +9039,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI63">
+  <conditionalFormatting sqref="A2:AI68">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>